<commit_message>
Correction of append error
</commit_message>
<xml_diff>
--- a/Grille_conso_elec.xlsx
+++ b/Grille_conso_elec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louau\Projets\Ademe_RCP_FAI\modele-rcp-fai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aubet Louise\Nextcloud\Drive_Partagé\60-69 Tech\62 LCA (specific FU)\62.08 ADEME RCP FAI\Archives\Modèle\Input\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D921CC1-F6B7-452A-AF33-1C6B59E79B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA38B60-F81B-4DE3-8B02-C5A15408EB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -927,6 +925,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,18 +981,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1266,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32657AA7-A293-41FC-8E8B-58993E82175E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1284,21 +1282,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="60" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="60" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="58"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9" ht="51.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1336,16 +1334,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="58" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="52" t="s">
+        <v>3504</v>
+      </c>
+      <c r="D3" s="56" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="27" t="s">
@@ -1354,7 +1352,7 @@
       <c r="F3" s="21">
         <v>0</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="56" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="27" t="s">
@@ -1365,193 +1363,193 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>98</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="25" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="15">
-        <v>0</v>
+        <v>6132</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="53"/>
+        <v>3504</v>
+      </c>
+      <c r="D5" s="57"/>
       <c r="E5" s="25" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="15">
-        <v>0</v>
+        <v>23652</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5">
         <v>82</v>
       </c>
-      <c r="D6" s="53"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
       </c>
-      <c r="G6" s="53"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="25" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="15">
-        <v>0</v>
+        <v>23652</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="5">
         <v>82</v>
       </c>
-      <c r="D7" s="53"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="25" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
       </c>
-      <c r="G7" s="53"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="25" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="15">
-        <v>0</v>
+        <v>23652</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="5">
         <v>35.04</v>
       </c>
-      <c r="D8" s="53"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="25" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
       </c>
-      <c r="G8" s="53"/>
+      <c r="G8" s="57"/>
       <c r="H8" s="25" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="15">
-        <v>0</v>
+        <v>23652</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="53"/>
+        <v>9127.92</v>
+      </c>
+      <c r="D9" s="57"/>
       <c r="E9" s="25" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="G9" s="53"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="25" t="s">
         <v>30</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>4248.6000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="55"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="5">
         <v>82</v>
       </c>
-      <c r="D10" s="53"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
       </c>
-      <c r="G10" s="53"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="25" t="s">
         <v>33</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>381.06</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="5">
         <v>0</v>
       </c>
-      <c r="D11" s="59"/>
+      <c r="D11" s="63"/>
       <c r="E11" s="26" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
       </c>
-      <c r="G11" s="62" t="s">
+      <c r="G11" s="66" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>36</v>
       </c>
       <c r="I11" s="36">
-        <v>0</v>
+        <v>4905.6000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="10" t="s">
         <v>37</v>
       </c>
@@ -1567,16 +1565,16 @@
       <c r="F12" s="46">
         <v>0</v>
       </c>
-      <c r="G12" s="63"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="25" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="15">
-        <v>0</v>
+        <v>97761.600000000006</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="10" t="s">
         <v>79</v>
       </c>
@@ -1592,16 +1590,16 @@
       <c r="F13" s="46">
         <v>0</v>
       </c>
-      <c r="G13" s="64"/>
+      <c r="G13" s="68"/>
       <c r="H13" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="37">
-        <v>0</v>
+        <v>18921.599999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="10" t="s">
         <v>80</v>
       </c>
@@ -1617,18 +1615,18 @@
       <c r="F14" s="42">
         <v>0</v>
       </c>
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="66" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="15">
-        <v>0</v>
+        <v>18921.599999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="10" t="s">
         <v>82</v>
       </c>
@@ -1638,16 +1636,16 @@
       <c r="D15" s="47"/>
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="63"/>
+      <c r="G15" s="67"/>
       <c r="H15" s="25" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="15">
-        <v>0</v>
+        <v>231264</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="10" t="s">
         <v>83</v>
       </c>
@@ -1657,96 +1655,96 @@
       <c r="D16" s="47"/>
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="63"/>
+      <c r="G16" s="67"/>
       <c r="H16" s="28" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="15">
-        <v>0</v>
+        <v>34886.699999999997</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="54" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="20">
-        <v>0</v>
+        <v>97761.600000000006</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="10"/>
       <c r="F17" s="39"/>
-      <c r="G17" s="63"/>
+      <c r="G17" s="67"/>
       <c r="H17" s="25" t="s">
         <v>42</v>
       </c>
       <c r="I17" s="15">
-        <v>0</v>
+        <v>13006.848</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="51"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="22">
-        <v>0</v>
+        <v>18921.599999999999</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="10"/>
       <c r="F18" s="39"/>
-      <c r="G18" s="63"/>
+      <c r="G18" s="67"/>
       <c r="H18" s="25" t="s">
         <v>45</v>
       </c>
       <c r="I18" s="15">
-        <v>0</v>
+        <v>16065.84</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="5">
-        <v>0</v>
+        <v>18921.599999999999</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="63"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="25" t="s">
         <v>48</v>
       </c>
       <c r="I19" s="15">
-        <v>0</v>
+        <v>13006.848</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="51"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>231264</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="63"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="25" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="15">
-        <v>0</v>
+        <v>97761.600000000006</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1758,16 +1756,16 @@
       <c r="D21" s="23"/>
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="64"/>
+      <c r="G21" s="68"/>
       <c r="H21" s="26" t="s">
         <v>53</v>
       </c>
       <c r="I21" s="15">
-        <v>0</v>
+        <v>381.06</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="66"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="12" t="s">
         <v>43</v>
       </c>
@@ -1777,7 +1775,7 @@
       <c r="D22" s="23"/>
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="65" t="s">
+      <c r="G22" s="50" t="s">
         <v>54</v>
       </c>
       <c r="H22" s="25" t="s">
@@ -1788,7 +1786,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="67"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="13" t="s">
         <v>46</v>
       </c>
@@ -1798,7 +1796,7 @@
       <c r="D23" s="23"/>
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="66"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="29" t="s">
         <v>56</v>
       </c>
@@ -1807,7 +1805,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="50" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -1819,7 +1817,7 @@
       <c r="D24" s="23"/>
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="66"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="29" t="s">
         <v>58</v>
       </c>
@@ -1828,7 +1826,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="66"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="12" t="s">
         <v>43</v>
       </c>
@@ -1838,7 +1836,7 @@
       <c r="D25" s="23"/>
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="66"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="48" t="s">
         <v>60</v>
       </c>
@@ -1847,7 +1845,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="66"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="12" t="s">
         <v>46</v>
       </c>
@@ -1857,7 +1855,7 @@
       <c r="D26" s="16"/>
       <c r="E26" s="15"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="67"/>
+      <c r="G26" s="52"/>
       <c r="H26" s="48" t="s">
         <v>62</v>
       </c>
@@ -1866,7 +1864,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="66"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="12" t="s">
         <v>55</v>
       </c>
@@ -1876,7 +1874,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="15"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="65" t="s">
+      <c r="G27" s="50" t="s">
         <v>74</v>
       </c>
       <c r="H27" s="24" t="s">
@@ -1887,7 +1885,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="66"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="12" t="s">
         <v>57</v>
       </c>
@@ -1897,7 +1895,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="15"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="66"/>
+      <c r="G28" s="51"/>
       <c r="H28" s="29" t="s">
         <v>56</v>
       </c>
@@ -1906,7 +1904,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="66"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="12" t="s">
         <v>59</v>
       </c>
@@ -1916,7 +1914,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="15"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="67"/>
+      <c r="G29" s="52"/>
       <c r="H29" s="49" t="s">
         <v>58</v>
       </c>
@@ -1925,7 +1923,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="66"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="12" t="s">
         <v>61</v>
       </c>
@@ -1935,7 +1933,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="15"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="65" t="s">
+      <c r="G30" s="50" t="s">
         <v>75</v>
       </c>
       <c r="H30" s="24" t="s">
@@ -1946,7 +1944,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="66"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="12" t="s">
         <v>62</v>
       </c>
@@ -1956,7 +1954,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="15"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="66"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="29" t="s">
         <v>56</v>
       </c>
@@ -1965,7 +1963,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="66"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="12" t="s">
         <v>63</v>
       </c>
@@ -1975,7 +1973,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="15"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="67"/>
+      <c r="G32" s="52"/>
       <c r="H32" s="49" t="s">
         <v>58</v>
       </c>
@@ -1984,7 +1982,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="66"/>
+      <c r="A33" s="51"/>
       <c r="B33" s="12" t="s">
         <v>64</v>
       </c>
@@ -1997,7 +1995,7 @@
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="67"/>
+      <c r="A34" s="52"/>
       <c r="B34" s="13" t="s">
         <v>65</v>
       </c>
@@ -2010,7 +2008,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="50" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -2025,7 +2023,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="66"/>
+      <c r="A36" s="51"/>
       <c r="B36" s="12" t="s">
         <v>43</v>
       </c>
@@ -2038,7 +2036,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="66"/>
+      <c r="A37" s="51"/>
       <c r="B37" s="12" t="s">
         <v>46</v>
       </c>
@@ -2053,7 +2051,7 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="66"/>
+      <c r="A38" s="51"/>
       <c r="B38" s="12" t="s">
         <v>55</v>
       </c>
@@ -2068,7 +2066,7 @@
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="66"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="12" t="s">
         <v>68</v>
       </c>
@@ -2083,7 +2081,7 @@
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="66"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="12" t="s">
         <v>59</v>
       </c>
@@ -2098,7 +2096,7 @@
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="66"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="12" t="s">
         <v>61</v>
       </c>
@@ -2113,7 +2111,7 @@
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="66"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="12" t="s">
         <v>62</v>
       </c>
@@ -2128,7 +2126,7 @@
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="66"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="12" t="s">
         <v>63</v>
       </c>
@@ -2143,7 +2141,7 @@
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="66"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="12" t="s">
         <v>64</v>
       </c>
@@ -2158,7 +2156,7 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="66"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="12" t="s">
         <v>65</v>
       </c>
@@ -2173,7 +2171,7 @@
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="66"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="12" t="s">
         <v>69</v>
       </c>
@@ -2188,7 +2186,7 @@
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="66"/>
+      <c r="A47" s="51"/>
       <c r="B47" s="12" t="s">
         <v>70</v>
       </c>
@@ -2203,7 +2201,7 @@
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="66"/>
+      <c r="A48" s="51"/>
       <c r="B48" s="12" t="s">
         <v>71</v>
       </c>
@@ -2218,7 +2216,7 @@
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="68"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="14" t="s">
         <v>72</v>
       </c>
@@ -2234,13 +2232,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="A35:A49"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A34"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="G3:G10"/>
     <mergeCell ref="A3:A16"/>
@@ -2250,6 +2241,13 @@
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="G14:G21"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="A35:A49"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>